<commit_message>
ML code version 1.2
</commit_message>
<xml_diff>
--- a/Code/ML versions.xlsx
+++ b/Code/ML versions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="70">
   <si>
     <t>Nx/Ox</t>
   </si>
@@ -208,6 +208,24 @@
   </si>
   <si>
     <t>Cross-validation</t>
+  </si>
+  <si>
+    <t>a27d7ad</t>
+  </si>
+  <si>
+    <t>Split before normalization</t>
+  </si>
+  <si>
+    <t>Correlated vfeatures</t>
+  </si>
+  <si>
+    <t>Bandgap, eV','Calc time (h)', 'Promoter, w%', 'Surface area, m2/g','CatW, g/L', 'Alcohol, %','Power, W', 'Wave length min, nm', 'Temperature, K'</t>
+  </si>
+  <si>
+    <t>Drop, 0.9  ['Wave length min, nm', 'Temperature, K', 'avg p valence electrons', 'frac f valence electrons', 'Promoter_Pt', 'Cell aterial_quartz']</t>
+  </si>
+  <si>
+    <t>1710c85</t>
   </si>
 </sst>
 </file>
@@ -251,7 +269,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +336,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -331,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -356,6 +380,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -663,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB21"/>
+  <dimension ref="A1:BC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AO23" sqref="AO23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,11 +703,11 @@
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="29" max="29" width="11.109375" customWidth="1"/>
-    <col min="40" max="40" width="13.77734375" customWidth="1"/>
-    <col min="41" max="42" width="10.44140625" customWidth="1"/>
+    <col min="40" max="41" width="13.77734375" customWidth="1"/>
+    <col min="42" max="43" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
@@ -726,28 +755,29 @@
       <c r="AL1" s="12"/>
       <c r="AM1" s="12"/>
       <c r="AN1" s="12"/>
-      <c r="AO1" s="14" t="s">
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14" t="s">
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="AR1" s="14"/>
       <c r="AS1" s="14"/>
       <c r="AT1" s="14"/>
       <c r="AU1" s="14"/>
       <c r="AV1" s="14"/>
-      <c r="AW1" s="14" t="s">
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="AX1" s="14"/>
       <c r="AY1" s="14"/>
       <c r="AZ1" s="14"/>
       <c r="BA1" s="14"/>
       <c r="BB1" s="14"/>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="BC1" s="14"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -866,50 +896,59 @@
       <c r="AN2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AO2" s="14" t="s">
+      <c r="AO2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AP2" s="14" t="s">
+      <c r="AQ2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AQ2" s="14" t="s">
+      <c r="AR2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AS2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AS2" s="14" t="s">
+      <c r="AT2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="AU2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AU2" s="14" t="s">
+      <c r="AV2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AV2" s="14" t="s">
+      <c r="AW2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="AX2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="AY2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AY2" s="14" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AZ2" s="14" t="s">
+      <c r="BA2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BA2" s="14" t="s">
+      <c r="BB2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="BB2" s="14" t="s">
+      <c r="BC2" s="14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
       <c r="C3">
         <v>1086</v>
       </c>
@@ -1022,31 +1061,46 @@
         <v>49</v>
       </c>
       <c r="AO3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AQ3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AQ3" s="13">
+      <c r="AR3" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>0.59</v>
       </c>
-      <c r="AS3" s="13">
+      <c r="AT3" s="13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AT3" s="13">
+      <c r="AU3" s="13">
         <v>0.81</v>
       </c>
-      <c r="AU3" s="13">
+      <c r="AV3" s="13">
         <v>0.78</v>
       </c>
-      <c r="AV3" s="15">
+      <c r="AW3" s="15">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX3" s="18"/>
+      <c r="AY3" s="18"/>
+      <c r="AZ3" s="18"/>
+      <c r="BA3" s="18"/>
+      <c r="BB3" s="18"/>
+      <c r="BC3" s="18"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
       <c r="C4">
         <v>1086</v>
       </c>
@@ -1159,71 +1213,584 @@
         <v>49</v>
       </c>
       <c r="AO4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AP4" s="11" t="s">
+      <c r="AQ4" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="AP5" t="s">
+      <c r="AR4">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="AS4">
+        <v>0.38</v>
+      </c>
+      <c r="AT4">
+        <v>0.61</v>
+      </c>
+      <c r="AU4">
+        <v>0.79</v>
+      </c>
+      <c r="AV4" s="16">
+        <v>0.99</v>
+      </c>
+      <c r="AW4">
+        <v>0.98</v>
+      </c>
+      <c r="AX4" s="18">
+        <v>1.98</v>
+      </c>
+      <c r="AY4" s="18">
+        <v>2.27</v>
+      </c>
+      <c r="AZ4" s="18">
+        <v>1.73</v>
+      </c>
+      <c r="BA4" s="18">
+        <v>1.31</v>
+      </c>
+      <c r="BB4" s="18">
+        <v>0.31</v>
+      </c>
+      <c r="BC4" s="18">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>1086</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="R5" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S5" s="6">
+        <v>-1</v>
+      </c>
+      <c r="T5" s="6">
+        <v>-1</v>
+      </c>
+      <c r="U5">
+        <v>745</v>
+      </c>
+      <c r="W5" s="6">
+        <v>745</v>
+      </c>
+      <c r="X5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5">
+        <v>745</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>665</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AR5">
+        <v>-0.11</v>
+      </c>
+      <c r="AS5">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="AT5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AU5">
+        <v>0.33</v>
+      </c>
+      <c r="AV5">
+        <v>0.19</v>
+      </c>
+      <c r="AW5">
+        <v>0.4</v>
+      </c>
+      <c r="AX5" s="18">
+        <v>3.11</v>
+      </c>
+      <c r="AY5" s="18">
+        <v>3.37</v>
+      </c>
+      <c r="AZ5" s="18">
+        <v>2.48</v>
+      </c>
+      <c r="BA5" s="18">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="BB5" s="18">
+        <v>2.66</v>
+      </c>
+      <c r="BC5" s="18">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>1086</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="R6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="T6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="U6">
+        <v>745</v>
+      </c>
+      <c r="W6" s="6">
+        <v>745</v>
+      </c>
+      <c r="X6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z6">
+        <v>745</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>665</v>
+      </c>
+      <c r="AH6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR6">
+        <v>-1.36</v>
+      </c>
+      <c r="AS6">
+        <v>0.11</v>
+      </c>
+      <c r="AT6">
+        <v>0.39</v>
+      </c>
+      <c r="AU6">
+        <v>0.47</v>
+      </c>
+      <c r="AV6">
+        <v>0.31</v>
+      </c>
+      <c r="AX6" s="18">
+        <v>4.49</v>
+      </c>
+      <c r="AY6" s="18">
+        <v>2.76</v>
+      </c>
+      <c r="AZ6" s="18">
+        <v>2.27</v>
+      </c>
+      <c r="BA6" s="18">
+        <v>2.13</v>
+      </c>
+      <c r="BB6" s="18">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="BC6" s="18"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="Y7" s="2"/>
+      <c r="AX7" s="18"/>
+      <c r="AY7" s="18"/>
+      <c r="AZ7" s="18"/>
+      <c r="BA7" s="18"/>
+      <c r="BB7" s="18"/>
+      <c r="BC7" s="18"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="Y8" s="2"/>
+      <c r="AP8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX8" s="18"/>
+      <c r="AY8" s="18"/>
+      <c r="AZ8" s="18"/>
+      <c r="BA8" s="18"/>
+      <c r="BB8" s="18"/>
+      <c r="BC8" s="18"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="Y9" s="2"/>
+      <c r="AX9" s="18"/>
+      <c r="AY9" s="18"/>
+      <c r="AZ9" s="18"/>
+      <c r="BA9" s="18"/>
+      <c r="BB9" s="18"/>
+      <c r="BC9" s="18"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX10" s="18"/>
+      <c r="AY10" s="18"/>
+      <c r="AZ10" s="18"/>
+      <c r="BA10" s="18"/>
+      <c r="BB10" s="18"/>
+      <c r="BC10" s="18"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX11" s="18"/>
+      <c r="AY11" s="18"/>
+      <c r="AZ11" s="18"/>
+      <c r="BA11" s="18"/>
+      <c r="BB11" s="18"/>
+      <c r="BC11" s="18"/>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX12" s="18"/>
+      <c r="AY12" s="18"/>
+      <c r="AZ12" s="18"/>
+      <c r="BA12" s="18"/>
+      <c r="BB12" s="18"/>
+      <c r="BC12" s="18"/>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX13" s="18"/>
+      <c r="AY13" s="18"/>
+      <c r="AZ13" s="18"/>
+      <c r="BA13" s="18"/>
+      <c r="BB13" s="18"/>
+      <c r="BC13" s="18"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX14" s="18"/>
+      <c r="AY14" s="18"/>
+      <c r="AZ14" s="18"/>
+      <c r="BA14" s="18"/>
+      <c r="BB14" s="18"/>
+      <c r="BC14" s="18"/>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AX15" s="18"/>
+      <c r="AY15" s="18"/>
+      <c r="AZ15" s="18"/>
+      <c r="BA15" s="18"/>
+      <c r="BB15" s="18"/>
+      <c r="BC15" s="18"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="AX16" s="18"/>
+      <c r="AY16" s="18"/>
+      <c r="AZ16" s="18"/>
+      <c r="BA16" s="18"/>
+      <c r="BB16" s="18"/>
+      <c r="BC16" s="18"/>
+    </row>
+    <row r="17" spans="11:55" x14ac:dyDescent="0.3">
       <c r="K17" s="1"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="AX17" s="18"/>
+      <c r="AY17" s="18"/>
+      <c r="AZ17" s="18"/>
+      <c r="BA17" s="18"/>
+      <c r="BB17" s="18"/>
+      <c r="BC17" s="18"/>
+    </row>
+    <row r="18" spans="11:55" x14ac:dyDescent="0.3">
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="AX18" s="18"/>
+      <c r="AY18" s="18"/>
+      <c r="AZ18" s="18"/>
+      <c r="BA18" s="18"/>
+      <c r="BB18" s="18"/>
+      <c r="BC18" s="18"/>
+    </row>
+    <row r="19" spans="11:55" x14ac:dyDescent="0.3">
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="AX19" s="18"/>
+      <c r="AY19" s="18"/>
+      <c r="AZ19" s="18"/>
+      <c r="BA19" s="18"/>
+      <c r="BB19" s="18"/>
+      <c r="BC19" s="18"/>
+    </row>
+    <row r="20" spans="11:55" x14ac:dyDescent="0.3">
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="AX20" s="18"/>
+      <c r="AY20" s="18"/>
+      <c r="AZ20" s="18"/>
+      <c r="BA20" s="18"/>
+      <c r="BB20" s="18"/>
+      <c r="BC20" s="18"/>
+    </row>
+    <row r="21" spans="11:55" x14ac:dyDescent="0.3">
       <c r="K21" s="2"/>
+      <c r="AX21" s="18"/>
+      <c r="AY21" s="18"/>
+      <c r="AZ21" s="18"/>
+      <c r="BA21" s="18"/>
+      <c r="BB21" s="18"/>
+      <c r="BC21" s="18"/>
+    </row>
+    <row r="22" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX22" s="18"/>
+      <c r="AY22" s="18"/>
+      <c r="AZ22" s="18"/>
+      <c r="BA22" s="18"/>
+      <c r="BB22" s="18"/>
+      <c r="BC22" s="18"/>
+    </row>
+    <row r="23" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX23" s="18"/>
+      <c r="AY23" s="18"/>
+      <c r="AZ23" s="18"/>
+      <c r="BA23" s="18"/>
+      <c r="BB23" s="18"/>
+      <c r="BC23" s="18"/>
+    </row>
+    <row r="24" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX24" s="18"/>
+      <c r="AY24" s="18"/>
+      <c r="AZ24" s="18"/>
+      <c r="BA24" s="18"/>
+      <c r="BB24" s="18"/>
+      <c r="BC24" s="18"/>
+    </row>
+    <row r="25" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX25" s="18"/>
+      <c r="AY25" s="18"/>
+      <c r="AZ25" s="18"/>
+      <c r="BA25" s="18"/>
+      <c r="BB25" s="18"/>
+      <c r="BC25" s="18"/>
+    </row>
+    <row r="26" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX26" s="18"/>
+      <c r="AY26" s="18"/>
+      <c r="AZ26" s="18"/>
+      <c r="BA26" s="18"/>
+      <c r="BB26" s="18"/>
+      <c r="BC26" s="18"/>
+    </row>
+    <row r="27" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX27" s="18"/>
+      <c r="AY27" s="18"/>
+      <c r="AZ27" s="18"/>
+      <c r="BA27" s="18"/>
+      <c r="BB27" s="18"/>
+      <c r="BC27" s="18"/>
+    </row>
+    <row r="28" spans="11:55" x14ac:dyDescent="0.3">
+      <c r="AX28" s="18"/>
+      <c r="AY28" s="18"/>
+      <c r="AZ28" s="18"/>
+      <c r="BA28" s="18"/>
+      <c r="BB28" s="18"/>
+      <c r="BC28" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Basic CIF modifier is added
</commit_message>
<xml_diff>
--- a/Code/ML versions.xlsx
+++ b/Code/ML versions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="82">
   <si>
     <t>Nx/Ox</t>
   </si>
@@ -238,6 +238,30 @@
   </si>
   <si>
     <t>89802a5</t>
+  </si>
+  <si>
+    <t>4872abc</t>
+  </si>
+  <si>
+    <t>Sac Agents</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>d9a6622</t>
+  </si>
+  <si>
+    <t>Bandgap, eV','Calc time (h)',, 'Temperature, K'</t>
+  </si>
+  <si>
+    <t>Drop, 0.9 ['Wave length min, nm', 'Temperature, K', 'frac f alence electrons', 'Promoter_Pt', 'Promoter_RuO2']</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Log_rate</t>
   </si>
 </sst>
 </file>
@@ -704,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD28"/>
+  <dimension ref="A1:BG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AN26" sqref="AN26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,11 +739,11 @@
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="30" max="30" width="11.109375" customWidth="1"/>
-    <col min="41" max="42" width="13.77734375" customWidth="1"/>
-    <col min="43" max="44" width="10.44140625" customWidth="1"/>
+    <col min="42" max="45" width="13.77734375" customWidth="1"/>
+    <col min="46" max="47" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
@@ -759,38 +783,41 @@
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
       <c r="AH1" s="7"/>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" s="12"/>
       <c r="AK1" s="12"/>
       <c r="AL1" s="12"/>
       <c r="AM1" s="12"/>
       <c r="AN1" s="12"/>
       <c r="AO1" s="12"/>
       <c r="AP1" s="12"/>
-      <c r="AQ1" s="14" t="s">
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14" t="s">
-        <v>59</v>
-      </c>
+      <c r="AS1" s="14"/>
       <c r="AT1" s="14"/>
       <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
+      <c r="AV1" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="AW1" s="14"/>
       <c r="AX1" s="14"/>
-      <c r="AY1" s="14" t="s">
-        <v>62</v>
-      </c>
+      <c r="AY1" s="14"/>
       <c r="AZ1" s="14"/>
       <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
+      <c r="BB1" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="BC1" s="14"/>
       <c r="BD1" s="14"/>
-    </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="14"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -889,76 +916,85 @@
         <v>39</v>
       </c>
       <c r="AH2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AJ2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AK2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AK2" s="12" t="s">
+      <c r="AL2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AL2" s="12" t="s">
+      <c r="AM2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AN2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AN2" s="12" t="s">
+      <c r="AO2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AO2" s="12" t="s">
+      <c r="AP2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AQ2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AQ2" s="14" t="s">
+      <c r="AR2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS2" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AU2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AS2" s="14" t="s">
+      <c r="AV2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="AW2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AU2" s="14" t="s">
+      <c r="AX2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AV2" s="14" t="s">
+      <c r="AY2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="BA2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AY2" s="14" t="s">
+      <c r="BB2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="14" t="s">
+      <c r="BC2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="BA2" s="14" t="s">
+      <c r="BD2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BB2" s="14" t="s">
+      <c r="BE2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BC2" s="14" t="s">
+      <c r="BF2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="BD2" s="14" t="s">
+      <c r="BG2" s="14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1055,15 +1091,15 @@
       <c r="AG3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AH3">
+      <c r="AH3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI3">
         <v>665</v>
       </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AJ3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AJ3" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="AK3" s="11" t="s">
         <v>32</v>
       </c>
@@ -1077,43 +1113,50 @@
         <v>32</v>
       </c>
       <c r="AO3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AQ3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AR3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="11" t="s">
+      <c r="AU3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AS3" s="13">
+      <c r="AV3" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AT3">
+      <c r="AW3">
         <v>0.59</v>
       </c>
-      <c r="AU3" s="13">
+      <c r="AX3" s="13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AV3" s="13">
+      <c r="AY3" s="13">
         <v>0.81</v>
       </c>
-      <c r="AW3" s="13">
+      <c r="AZ3" s="13">
         <v>0.78</v>
       </c>
-      <c r="AX3" s="15">
+      <c r="BA3" s="15">
         <v>0.84</v>
       </c>
-      <c r="AY3" s="18"/>
-      <c r="AZ3" s="18"/>
-      <c r="BA3" s="18"/>
       <c r="BB3" s="18"/>
       <c r="BC3" s="18"/>
       <c r="BD3" s="18"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE3" s="18"/>
+      <c r="BF3" s="18"/>
+      <c r="BG3" s="18"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1210,15 +1253,15 @@
       <c r="AG4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI4">
         <v>665</v>
       </c>
-      <c r="AI4" s="11" t="s">
+      <c r="AJ4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AJ4" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="AK4" s="11" t="s">
         <v>32</v>
       </c>
@@ -1232,55 +1275,62 @@
         <v>32</v>
       </c>
       <c r="AO4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AP4" s="11" t="s">
+      <c r="AQ4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AQ4" s="11" t="s">
+      <c r="AR4" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS4" s="11"/>
+      <c r="AT4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AR4" s="11" t="s">
+      <c r="AU4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AS4">
+      <c r="AV4">
         <v>0.52800000000000002</v>
       </c>
-      <c r="AT4">
+      <c r="AW4">
         <v>0.38</v>
       </c>
-      <c r="AU4">
+      <c r="AX4">
         <v>0.61</v>
       </c>
-      <c r="AV4">
+      <c r="AY4">
         <v>0.79</v>
       </c>
-      <c r="AW4" s="16">
+      <c r="AZ4" s="16">
         <v>0.99</v>
       </c>
-      <c r="AX4">
+      <c r="BA4">
         <v>0.98</v>
       </c>
-      <c r="AY4" s="18">
+      <c r="BB4" s="18">
         <v>1.98</v>
       </c>
-      <c r="AZ4" s="18">
+      <c r="BC4" s="18">
         <v>2.27</v>
       </c>
-      <c r="BA4" s="18">
+      <c r="BD4" s="18">
         <v>1.73</v>
       </c>
-      <c r="BB4" s="18">
+      <c r="BE4" s="18">
         <v>1.31</v>
       </c>
-      <c r="BC4" s="18">
+      <c r="BF4" s="18">
         <v>0.31</v>
       </c>
-      <c r="BD4" s="18">
+      <c r="BG4" s="18">
         <v>0.39</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1377,15 +1427,15 @@
       <c r="AG5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AH5">
+      <c r="AH5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI5">
         <v>665</v>
       </c>
-      <c r="AI5" s="11" t="s">
+      <c r="AJ5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AJ5" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="AK5" s="11" t="s">
         <v>32</v>
       </c>
@@ -1399,55 +1449,62 @@
         <v>32</v>
       </c>
       <c r="AO5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AP5" s="11" t="s">
+      <c r="AQ5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AQ5" s="11" t="s">
+      <c r="AR5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS5" s="11"/>
+      <c r="AT5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AU5" t="s">
         <v>63</v>
       </c>
-      <c r="AS5">
+      <c r="AV5">
         <v>-0.11</v>
       </c>
-      <c r="AT5">
+      <c r="AW5">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="AU5">
+      <c r="AX5">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AV5">
+      <c r="AY5">
         <v>0.33</v>
       </c>
-      <c r="AW5">
+      <c r="AZ5">
         <v>0.19</v>
       </c>
-      <c r="AX5">
+      <c r="BA5">
         <v>0.4</v>
       </c>
-      <c r="AY5" s="18">
+      <c r="BB5" s="18">
         <v>3.11</v>
       </c>
-      <c r="AZ5" s="18">
+      <c r="BC5" s="18">
         <v>3.37</v>
       </c>
-      <c r="BA5" s="18">
+      <c r="BD5" s="18">
         <v>2.48</v>
       </c>
-      <c r="BB5" s="18">
+      <c r="BE5" s="18">
         <v>2.4300000000000002</v>
       </c>
-      <c r="BC5" s="18">
+      <c r="BF5" s="18">
         <v>2.66</v>
       </c>
-      <c r="BD5" s="18">
+      <c r="BG5" s="18">
         <v>2.27</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1544,15 +1601,15 @@
       <c r="AG6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AH6">
+      <c r="AH6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI6">
         <v>305</v>
       </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AJ6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AJ6" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="AK6" s="11" t="s">
         <v>32</v>
       </c>
@@ -1566,55 +1623,62 @@
         <v>32</v>
       </c>
       <c r="AO6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AP6" s="11" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="AQ6" s="11" t="s">
+      <c r="AR6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AU6" t="s">
         <v>63</v>
       </c>
-      <c r="AS6">
+      <c r="AV6">
         <v>-1.36</v>
       </c>
-      <c r="AT6">
+      <c r="AW6">
         <v>0.11</v>
       </c>
-      <c r="AU6">
+      <c r="AX6">
         <v>0.39</v>
       </c>
-      <c r="AV6">
+      <c r="AY6">
         <v>0.47</v>
       </c>
-      <c r="AW6">
+      <c r="AZ6">
         <v>0.31</v>
       </c>
-      <c r="AX6">
+      <c r="BA6">
         <v>0.52</v>
       </c>
-      <c r="AY6" s="18">
+      <c r="BB6" s="18">
         <v>4.49</v>
       </c>
-      <c r="AZ6" s="18">
+      <c r="BC6" s="18">
         <v>2.76</v>
       </c>
-      <c r="BA6" s="18">
+      <c r="BD6" s="18">
         <v>2.27</v>
       </c>
-      <c r="BB6" s="18">
+      <c r="BE6" s="18">
         <v>2.13</v>
       </c>
-      <c r="BC6" s="18">
+      <c r="BF6" s="18">
         <v>2.4300000000000002</v>
       </c>
-      <c r="BD6" s="18">
+      <c r="BG6" s="18">
         <v>2.02</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1711,15 +1775,15 @@
       <c r="AG7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AH7">
+      <c r="AH7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI7">
         <v>369</v>
       </c>
-      <c r="AI7" s="11" t="s">
+      <c r="AJ7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AJ7" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="AK7" s="11" t="s">
         <v>32</v>
       </c>
@@ -1733,270 +1797,753 @@
         <v>32</v>
       </c>
       <c r="AO7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AP7" s="11" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="AQ7" s="11" t="s">
+      <c r="AR7" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AU7" t="s">
         <v>63</v>
       </c>
-      <c r="AS7">
+      <c r="AV7">
         <v>-0.47</v>
       </c>
-      <c r="AT7">
+      <c r="AW7">
         <v>0.25</v>
       </c>
-      <c r="AU7">
+      <c r="AX7">
         <v>0.41</v>
       </c>
-      <c r="AV7">
+      <c r="AY7">
         <v>0.52</v>
       </c>
-      <c r="AW7">
+      <c r="AZ7">
         <v>0.35</v>
       </c>
-      <c r="AX7">
+      <c r="BA7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AY7" s="18">
+      <c r="BB7" s="18">
         <v>3.63</v>
       </c>
-      <c r="AZ7" s="18">
+      <c r="BC7" s="18">
         <v>2.58</v>
       </c>
-      <c r="BA7" s="18">
+      <c r="BD7" s="18">
         <v>2.2799999999999998</v>
       </c>
-      <c r="BB7" s="18">
+      <c r="BE7" s="18">
         <v>2.0699999999999998</v>
       </c>
-      <c r="BC7" s="18">
+      <c r="BF7" s="18">
         <v>2.4</v>
       </c>
-      <c r="BD7" s="18">
+      <c r="BG7" s="18">
         <v>1.99</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="Z8" s="2"/>
-      <c r="AY8" s="18"/>
-      <c r="AZ8" s="18"/>
-      <c r="BA8" s="18"/>
-      <c r="BB8" s="18"/>
-      <c r="BC8" s="18"/>
-      <c r="BD8" s="18"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AY9" s="18"/>
-      <c r="AZ9" s="18"/>
-      <c r="BA9" s="18"/>
-      <c r="BB9" s="18"/>
-      <c r="BC9" s="18"/>
-      <c r="BD9" s="18"/>
-    </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="AY10" s="18"/>
-      <c r="AZ10" s="18"/>
-      <c r="BA10" s="18"/>
-      <c r="BB10" s="18"/>
-      <c r="BC10" s="18"/>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>1086</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="S8" s="6">
+        <v>-1</v>
+      </c>
+      <c r="T8" s="6">
+        <v>-1</v>
+      </c>
+      <c r="U8" s="6">
+        <v>-1</v>
+      </c>
+      <c r="V8" s="11">
+        <v>968</v>
+      </c>
+      <c r="X8" s="11">
+        <v>968</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA8">
+        <v>406</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>378</v>
+      </c>
+      <c r="AJ8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS8" s="11">
+        <v>2.88</v>
+      </c>
+      <c r="AT8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV8">
+        <v>-0.7</v>
+      </c>
+      <c r="AW8">
+        <v>0.18</v>
+      </c>
+      <c r="AX8">
+        <v>0.39</v>
+      </c>
+      <c r="AY8">
+        <v>0.59</v>
+      </c>
+      <c r="AZ8">
+        <v>0.36</v>
+      </c>
+      <c r="BA8">
+        <v>0.63</v>
+      </c>
+      <c r="BB8" s="18">
+        <v>3.76</v>
+      </c>
+      <c r="BC8" s="18">
+        <v>2.61</v>
+      </c>
+      <c r="BD8" s="18">
+        <v>2.23</v>
+      </c>
+      <c r="BE8" s="18">
+        <v>1.83</v>
+      </c>
+      <c r="BF8" s="18">
+        <v>2.29</v>
+      </c>
+      <c r="BG8" s="18">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9">
+        <v>1086</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="S9" s="6">
+        <v>-1</v>
+      </c>
+      <c r="T9" s="6">
+        <v>-1</v>
+      </c>
+      <c r="U9" s="6">
+        <v>-1</v>
+      </c>
+      <c r="V9" s="11">
+        <v>968</v>
+      </c>
+      <c r="X9" s="11">
+        <v>968</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z9" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA9">
+        <v>669</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>574</v>
+      </c>
+      <c r="AJ9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS9" s="11">
+        <v>3.09</v>
+      </c>
+      <c r="AT9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV9">
+        <v>-1.39</v>
+      </c>
+      <c r="AW9">
+        <v>-0.17</v>
+      </c>
+      <c r="AX9">
+        <v>0.38</v>
+      </c>
+      <c r="AY9">
+        <v>0.46</v>
+      </c>
+      <c r="AZ9">
+        <v>0.3</v>
+      </c>
+      <c r="BA9">
+        <v>0.49</v>
+      </c>
+      <c r="BB9" s="18">
+        <v>4.78</v>
+      </c>
+      <c r="BC9" s="18">
+        <v>3.35</v>
+      </c>
+      <c r="BD9" s="18">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="BE9" s="18">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BF9" s="18">
+        <v>2.57</v>
+      </c>
+      <c r="BG9" s="18">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10">
+        <v>1086</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="6">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="S10" s="6">
+        <v>-1</v>
+      </c>
+      <c r="T10" s="6">
+        <v>-1</v>
+      </c>
+      <c r="U10" s="6">
+        <v>-1</v>
+      </c>
+      <c r="V10" s="11">
+        <v>968</v>
+      </c>
+      <c r="X10" s="11">
+        <v>968</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA10">
+        <v>406</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>385</v>
+      </c>
+      <c r="AJ10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS10" s="11">
+        <v>3.09</v>
+      </c>
+      <c r="AT10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV10">
+        <v>-1.43</v>
+      </c>
+      <c r="AW10">
+        <v>-0.13</v>
+      </c>
+      <c r="BB10" s="18">
+        <v>38596</v>
+      </c>
+      <c r="BC10" s="18">
+        <v>26237</v>
+      </c>
       <c r="BD10" s="18"/>
-    </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE10" s="18"/>
+      <c r="BF10" s="18"/>
+      <c r="BG10" s="18"/>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="AY11" s="18"/>
-      <c r="AZ11" s="18"/>
-      <c r="BA11" s="18"/>
       <c r="BB11" s="18"/>
       <c r="BC11" s="18"/>
       <c r="BD11" s="18"/>
-    </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE11" s="18"/>
+      <c r="BF11" s="18"/>
+      <c r="BG11" s="18"/>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="AY12" s="18"/>
-      <c r="AZ12" s="18"/>
-      <c r="BA12" s="18"/>
       <c r="BB12" s="18"/>
       <c r="BC12" s="18"/>
       <c r="BD12" s="18"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE12" s="18"/>
+      <c r="BF12" s="18"/>
+      <c r="BG12" s="18"/>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="AQ13" t="s">
+      <c r="AT13" t="s">
         <v>72</v>
       </c>
-      <c r="AY13" s="18"/>
-      <c r="AZ13" s="18"/>
-      <c r="BA13" s="18"/>
       <c r="BB13" s="18"/>
       <c r="BC13" s="18"/>
       <c r="BD13" s="18"/>
-    </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE13" s="18"/>
+      <c r="BF13" s="18"/>
+      <c r="BG13" s="18"/>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="AQ14" t="s">
+      <c r="AT14" t="s">
         <v>65</v>
       </c>
-      <c r="AY14" s="18"/>
-      <c r="AZ14" s="18"/>
-      <c r="BA14" s="18"/>
       <c r="BB14" s="18"/>
       <c r="BC14" s="18"/>
       <c r="BD14" s="18"/>
-    </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE14" s="18"/>
+      <c r="BF14" s="18"/>
+      <c r="BG14" s="18"/>
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="AY15" s="18"/>
-      <c r="AZ15" s="18"/>
-      <c r="BA15" s="18"/>
       <c r="BB15" s="18"/>
       <c r="BC15" s="18"/>
       <c r="BD15" s="18"/>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="BE15" s="18"/>
+      <c r="BF15" s="18"/>
+      <c r="BG15" s="18"/>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="AY16" s="18"/>
-      <c r="AZ16" s="18"/>
-      <c r="BA16" s="18"/>
       <c r="BB16" s="18"/>
       <c r="BC16" s="18"/>
       <c r="BD16" s="18"/>
-    </row>
-    <row r="17" spans="11:56" x14ac:dyDescent="0.3">
+      <c r="BE16" s="18"/>
+      <c r="BF16" s="18"/>
+      <c r="BG16" s="18"/>
+    </row>
+    <row r="17" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K17" s="1"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="AY17" s="18"/>
-      <c r="AZ17" s="18"/>
-      <c r="BA17" s="18"/>
       <c r="BB17" s="18"/>
       <c r="BC17" s="18"/>
       <c r="BD17" s="18"/>
-    </row>
-    <row r="18" spans="11:56" x14ac:dyDescent="0.3">
+      <c r="BE17" s="18"/>
+      <c r="BF17" s="18"/>
+      <c r="BG17" s="18"/>
+    </row>
+    <row r="18" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="AY18" s="18"/>
-      <c r="AZ18" s="18"/>
-      <c r="BA18" s="18"/>
       <c r="BB18" s="18"/>
       <c r="BC18" s="18"/>
       <c r="BD18" s="18"/>
-    </row>
-    <row r="19" spans="11:56" x14ac:dyDescent="0.3">
+      <c r="BE18" s="18"/>
+      <c r="BF18" s="18"/>
+      <c r="BG18" s="18"/>
+    </row>
+    <row r="19" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="AY19" s="18"/>
-      <c r="AZ19" s="18"/>
-      <c r="BA19" s="18"/>
       <c r="BB19" s="18"/>
       <c r="BC19" s="18"/>
       <c r="BD19" s="18"/>
-    </row>
-    <row r="20" spans="11:56" x14ac:dyDescent="0.3">
+      <c r="BE19" s="18"/>
+      <c r="BF19" s="18"/>
+      <c r="BG19" s="18"/>
+    </row>
+    <row r="20" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
-      <c r="AY20" s="18"/>
-      <c r="AZ20" s="18"/>
-      <c r="BA20" s="18"/>
       <c r="BB20" s="18"/>
       <c r="BC20" s="18"/>
       <c r="BD20" s="18"/>
-    </row>
-    <row r="21" spans="11:56" x14ac:dyDescent="0.3">
+      <c r="BE20" s="18"/>
+      <c r="BF20" s="18"/>
+      <c r="BG20" s="18"/>
+    </row>
+    <row r="21" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K21" s="2"/>
-      <c r="AY21" s="18"/>
-      <c r="AZ21" s="18"/>
-      <c r="BA21" s="18"/>
       <c r="BB21" s="18"/>
       <c r="BC21" s="18"/>
       <c r="BD21" s="18"/>
-    </row>
-    <row r="22" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY22" s="18"/>
-      <c r="AZ22" s="18"/>
-      <c r="BA22" s="18"/>
+      <c r="BE21" s="18"/>
+      <c r="BF21" s="18"/>
+      <c r="BG21" s="18"/>
+    </row>
+    <row r="22" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB22" s="18"/>
       <c r="BC22" s="18"/>
       <c r="BD22" s="18"/>
-    </row>
-    <row r="23" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY23" s="18"/>
-      <c r="AZ23" s="18"/>
-      <c r="BA23" s="18"/>
+      <c r="BE22" s="18"/>
+      <c r="BF22" s="18"/>
+      <c r="BG22" s="18"/>
+    </row>
+    <row r="23" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB23" s="18"/>
       <c r="BC23" s="18"/>
       <c r="BD23" s="18"/>
-    </row>
-    <row r="24" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY24" s="18"/>
-      <c r="AZ24" s="18"/>
-      <c r="BA24" s="18"/>
+      <c r="BE23" s="18"/>
+      <c r="BF23" s="18"/>
+      <c r="BG23" s="18"/>
+    </row>
+    <row r="24" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB24" s="18"/>
       <c r="BC24" s="18"/>
       <c r="BD24" s="18"/>
-    </row>
-    <row r="25" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY25" s="18"/>
-      <c r="AZ25" s="18"/>
-      <c r="BA25" s="18"/>
+      <c r="BE24" s="18"/>
+      <c r="BF24" s="18"/>
+      <c r="BG24" s="18"/>
+    </row>
+    <row r="25" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB25" s="18"/>
       <c r="BC25" s="18"/>
       <c r="BD25" s="18"/>
-    </row>
-    <row r="26" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY26" s="18"/>
-      <c r="AZ26" s="18"/>
-      <c r="BA26" s="18"/>
+      <c r="BE25" s="18"/>
+      <c r="BF25" s="18"/>
+      <c r="BG25" s="18"/>
+    </row>
+    <row r="26" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB26" s="18"/>
       <c r="BC26" s="18"/>
       <c r="BD26" s="18"/>
-    </row>
-    <row r="27" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY27" s="18"/>
-      <c r="AZ27" s="18"/>
-      <c r="BA27" s="18"/>
+      <c r="BE26" s="18"/>
+      <c r="BF26" s="18"/>
+      <c r="BG26" s="18"/>
+    </row>
+    <row r="27" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB27" s="18"/>
       <c r="BC27" s="18"/>
       <c r="BD27" s="18"/>
-    </row>
-    <row r="28" spans="11:56" x14ac:dyDescent="0.3">
-      <c r="AY28" s="18"/>
-      <c r="AZ28" s="18"/>
-      <c r="BA28" s="18"/>
+      <c r="BE27" s="18"/>
+      <c r="BF27" s="18"/>
+      <c r="BG27" s="18"/>
+    </row>
+    <row r="28" spans="11:59" x14ac:dyDescent="0.3">
       <c r="BB28" s="18"/>
       <c r="BC28" s="18"/>
       <c r="BD28" s="18"/>
+      <c r="BE28" s="18"/>
+      <c r="BF28" s="18"/>
+      <c r="BG28" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Almost all entries have a corresponding CIF file
</commit_message>
<xml_diff>
--- a/Code/ML versions.xlsx
+++ b/Code/ML versions.xlsx
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AM18" sqref="AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Basic strutiral featurizers are added
</commit_message>
<xml_diff>
--- a/Code/ML versions.xlsx
+++ b/Code/ML versions.xlsx
@@ -356,12 +356,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -375,6 +369,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,15 +412,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AM18" sqref="AM18"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AU5" sqref="AU5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,18 +1143,18 @@
       <c r="AY3" s="13">
         <v>0.81</v>
       </c>
-      <c r="AZ3" s="13">
+      <c r="AZ3" s="18">
         <v>0.78</v>
       </c>
-      <c r="BA3" s="15">
+      <c r="BA3" s="18">
         <v>0.84</v>
       </c>
-      <c r="BB3" s="18"/>
-      <c r="BC3" s="18"/>
-      <c r="BD3" s="18"/>
-      <c r="BE3" s="18"/>
-      <c r="BF3" s="18"/>
-      <c r="BG3" s="18"/>
+      <c r="BB3" s="16"/>
+      <c r="BC3" s="16"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="16"/>
+      <c r="BG3" s="16"/>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1305,28 +1305,28 @@
       <c r="AY4">
         <v>0.79</v>
       </c>
-      <c r="AZ4" s="16">
+      <c r="AZ4" s="11">
         <v>0.99</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="11">
         <v>0.98</v>
       </c>
-      <c r="BB4" s="18">
+      <c r="BB4" s="16">
         <v>1.98</v>
       </c>
-      <c r="BC4" s="18">
+      <c r="BC4" s="16">
         <v>2.27</v>
       </c>
-      <c r="BD4" s="18">
+      <c r="BD4" s="16">
         <v>1.73</v>
       </c>
-      <c r="BE4" s="18">
+      <c r="BE4" s="16">
         <v>1.31</v>
       </c>
-      <c r="BF4" s="18">
+      <c r="BF4" s="16">
         <v>0.31</v>
       </c>
-      <c r="BG4" s="18">
+      <c r="BG4" s="16">
         <v>0.39</v>
       </c>
     </row>
@@ -1485,22 +1485,22 @@
       <c r="BA5">
         <v>0.4</v>
       </c>
-      <c r="BB5" s="18">
+      <c r="BB5" s="16">
         <v>3.11</v>
       </c>
-      <c r="BC5" s="18">
+      <c r="BC5" s="16">
         <v>3.37</v>
       </c>
-      <c r="BD5" s="18">
+      <c r="BD5" s="16">
         <v>2.48</v>
       </c>
-      <c r="BE5" s="18">
+      <c r="BE5" s="16">
         <v>2.4300000000000002</v>
       </c>
-      <c r="BF5" s="18">
+      <c r="BF5" s="16">
         <v>2.66</v>
       </c>
-      <c r="BG5" s="18">
+      <c r="BG5" s="16">
         <v>2.27</v>
       </c>
     </row>
@@ -1577,7 +1577,7 @@
       <c r="Y6" t="s">
         <v>27</v>
       </c>
-      <c r="Z6" s="17" t="s">
+      <c r="Z6" s="15" t="s">
         <v>67</v>
       </c>
       <c r="AA6">
@@ -1659,22 +1659,22 @@
       <c r="BA6">
         <v>0.52</v>
       </c>
-      <c r="BB6" s="18">
+      <c r="BB6" s="16">
         <v>4.49</v>
       </c>
-      <c r="BC6" s="18">
+      <c r="BC6" s="16">
         <v>2.76</v>
       </c>
-      <c r="BD6" s="18">
+      <c r="BD6" s="16">
         <v>2.27</v>
       </c>
-      <c r="BE6" s="18">
+      <c r="BE6" s="16">
         <v>2.13</v>
       </c>
-      <c r="BF6" s="18">
+      <c r="BF6" s="16">
         <v>2.4300000000000002</v>
       </c>
-      <c r="BG6" s="18">
+      <c r="BG6" s="16">
         <v>2.02</v>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       <c r="Y7" t="s">
         <v>27</v>
       </c>
-      <c r="Z7" s="17" t="s">
+      <c r="Z7" s="15" t="s">
         <v>67</v>
       </c>
       <c r="AA7">
@@ -1833,22 +1833,22 @@
       <c r="BA7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="BB7" s="18">
+      <c r="BB7" s="16">
         <v>3.63</v>
       </c>
-      <c r="BC7" s="18">
+      <c r="BC7" s="16">
         <v>2.58</v>
       </c>
-      <c r="BD7" s="18">
+      <c r="BD7" s="16">
         <v>2.2799999999999998</v>
       </c>
-      <c r="BE7" s="18">
+      <c r="BE7" s="16">
         <v>2.0699999999999998</v>
       </c>
-      <c r="BF7" s="18">
+      <c r="BF7" s="16">
         <v>2.4</v>
       </c>
-      <c r="BG7" s="18">
+      <c r="BG7" s="16">
         <v>1.99</v>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       <c r="Y8" t="s">
         <v>27</v>
       </c>
-      <c r="Z8" s="17" t="s">
+      <c r="Z8" s="15" t="s">
         <v>67</v>
       </c>
       <c r="AA8">
@@ -1991,40 +1991,40 @@
       <c r="AU8" t="s">
         <v>63</v>
       </c>
-      <c r="AV8">
+      <c r="AV8" s="17">
         <v>-0.7</v>
       </c>
-      <c r="AW8">
+      <c r="AW8" s="17">
         <v>0.18</v>
       </c>
-      <c r="AX8">
+      <c r="AX8" s="17">
         <v>0.39</v>
       </c>
-      <c r="AY8">
+      <c r="AY8" s="17">
         <v>0.59</v>
       </c>
-      <c r="AZ8">
+      <c r="AZ8" s="17">
         <v>0.36</v>
       </c>
-      <c r="BA8">
+      <c r="BA8" s="17">
         <v>0.63</v>
       </c>
-      <c r="BB8" s="18">
+      <c r="BB8" s="17">
         <v>3.76</v>
       </c>
-      <c r="BC8" s="18">
+      <c r="BC8" s="17">
         <v>2.61</v>
       </c>
-      <c r="BD8" s="18">
+      <c r="BD8" s="17">
         <v>2.23</v>
       </c>
-      <c r="BE8" s="18">
+      <c r="BE8" s="17">
         <v>1.83</v>
       </c>
-      <c r="BF8" s="18">
+      <c r="BF8" s="17">
         <v>2.29</v>
       </c>
-      <c r="BG8" s="18">
+      <c r="BG8" s="17">
         <v>1.75</v>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       <c r="Y9" t="s">
         <v>27</v>
       </c>
-      <c r="Z9" s="17" t="s">
+      <c r="Z9" s="15" t="s">
         <v>78</v>
       </c>
       <c r="AA9">
@@ -2185,22 +2185,22 @@
       <c r="BA9">
         <v>0.49</v>
       </c>
-      <c r="BB9" s="18">
+      <c r="BB9" s="16">
         <v>4.78</v>
       </c>
-      <c r="BC9" s="18">
+      <c r="BC9" s="16">
         <v>3.35</v>
       </c>
-      <c r="BD9" s="18">
+      <c r="BD9" s="16">
         <v>2.4300000000000002</v>
       </c>
-      <c r="BE9" s="18">
+      <c r="BE9" s="16">
         <v>2.2599999999999998</v>
       </c>
-      <c r="BF9" s="18">
+      <c r="BF9" s="16">
         <v>2.57</v>
       </c>
-      <c r="BG9" s="18">
+      <c r="BG9" s="16">
         <v>2.19</v>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       <c r="Y10" t="s">
         <v>27</v>
       </c>
-      <c r="Z10" s="17" t="s">
+      <c r="Z10" s="15" t="s">
         <v>67</v>
       </c>
       <c r="AA10">
@@ -2349,38 +2349,38 @@
       <c r="AW10">
         <v>-0.13</v>
       </c>
-      <c r="BB10" s="18">
+      <c r="BB10" s="16">
         <v>38596</v>
       </c>
-      <c r="BC10" s="18">
+      <c r="BC10" s="16">
         <v>26237</v>
       </c>
-      <c r="BD10" s="18"/>
-      <c r="BE10" s="18"/>
-      <c r="BF10" s="18"/>
-      <c r="BG10" s="18"/>
+      <c r="BD10" s="16"/>
+      <c r="BE10" s="16"/>
+      <c r="BF10" s="16"/>
+      <c r="BG10" s="16"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="BB11" s="18"/>
-      <c r="BC11" s="18"/>
-      <c r="BD11" s="18"/>
-      <c r="BE11" s="18"/>
-      <c r="BF11" s="18"/>
-      <c r="BG11" s="18"/>
+      <c r="BB11" s="16"/>
+      <c r="BC11" s="16"/>
+      <c r="BD11" s="16"/>
+      <c r="BE11" s="16"/>
+      <c r="BF11" s="16"/>
+      <c r="BG11" s="16"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="BB12" s="18"/>
-      <c r="BC12" s="18"/>
-      <c r="BD12" s="18"/>
-      <c r="BE12" s="18"/>
-      <c r="BF12" s="18"/>
-      <c r="BG12" s="18"/>
+      <c r="BB12" s="16"/>
+      <c r="BC12" s="16"/>
+      <c r="BD12" s="16"/>
+      <c r="BE12" s="16"/>
+      <c r="BF12" s="16"/>
+      <c r="BG12" s="16"/>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L13" s="2"/>
@@ -2389,12 +2389,12 @@
       <c r="AT13" t="s">
         <v>72</v>
       </c>
-      <c r="BB13" s="18"/>
-      <c r="BC13" s="18"/>
-      <c r="BD13" s="18"/>
-      <c r="BE13" s="18"/>
-      <c r="BF13" s="18"/>
-      <c r="BG13" s="18"/>
+      <c r="BB13" s="16"/>
+      <c r="BC13" s="16"/>
+      <c r="BD13" s="16"/>
+      <c r="BE13" s="16"/>
+      <c r="BF13" s="16"/>
+      <c r="BG13" s="16"/>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L14" s="2"/>
@@ -2403,147 +2403,147 @@
       <c r="AT14" t="s">
         <v>65</v>
       </c>
-      <c r="BB14" s="18"/>
-      <c r="BC14" s="18"/>
-      <c r="BD14" s="18"/>
-      <c r="BE14" s="18"/>
-      <c r="BF14" s="18"/>
-      <c r="BG14" s="18"/>
+      <c r="BB14" s="16"/>
+      <c r="BC14" s="16"/>
+      <c r="BD14" s="16"/>
+      <c r="BE14" s="16"/>
+      <c r="BF14" s="16"/>
+      <c r="BG14" s="16"/>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="BB15" s="18"/>
-      <c r="BC15" s="18"/>
-      <c r="BD15" s="18"/>
-      <c r="BE15" s="18"/>
-      <c r="BF15" s="18"/>
-      <c r="BG15" s="18"/>
+      <c r="BB15" s="16"/>
+      <c r="BC15" s="16"/>
+      <c r="BD15" s="16"/>
+      <c r="BE15" s="16"/>
+      <c r="BF15" s="16"/>
+      <c r="BG15" s="16"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="BB16" s="18"/>
-      <c r="BC16" s="18"/>
-      <c r="BD16" s="18"/>
-      <c r="BE16" s="18"/>
-      <c r="BF16" s="18"/>
-      <c r="BG16" s="18"/>
+      <c r="BB16" s="16"/>
+      <c r="BC16" s="16"/>
+      <c r="BD16" s="16"/>
+      <c r="BE16" s="16"/>
+      <c r="BF16" s="16"/>
+      <c r="BG16" s="16"/>
     </row>
     <row r="17" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K17" s="1"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="BB17" s="18"/>
-      <c r="BC17" s="18"/>
-      <c r="BD17" s="18"/>
-      <c r="BE17" s="18"/>
-      <c r="BF17" s="18"/>
-      <c r="BG17" s="18"/>
+      <c r="BB17" s="16"/>
+      <c r="BC17" s="16"/>
+      <c r="BD17" s="16"/>
+      <c r="BE17" s="16"/>
+      <c r="BF17" s="16"/>
+      <c r="BG17" s="16"/>
     </row>
     <row r="18" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="BB18" s="18"/>
-      <c r="BC18" s="18"/>
-      <c r="BD18" s="18"/>
-      <c r="BE18" s="18"/>
-      <c r="BF18" s="18"/>
-      <c r="BG18" s="18"/>
+      <c r="BB18" s="16"/>
+      <c r="BC18" s="16"/>
+      <c r="BD18" s="16"/>
+      <c r="BE18" s="16"/>
+      <c r="BF18" s="16"/>
+      <c r="BG18" s="16"/>
     </row>
     <row r="19" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="BB19" s="18"/>
-      <c r="BC19" s="18"/>
-      <c r="BD19" s="18"/>
-      <c r="BE19" s="18"/>
-      <c r="BF19" s="18"/>
-      <c r="BG19" s="18"/>
+      <c r="BB19" s="16"/>
+      <c r="BC19" s="16"/>
+      <c r="BD19" s="16"/>
+      <c r="BE19" s="16"/>
+      <c r="BF19" s="16"/>
+      <c r="BG19" s="16"/>
     </row>
     <row r="20" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
-      <c r="BB20" s="18"/>
-      <c r="BC20" s="18"/>
-      <c r="BD20" s="18"/>
-      <c r="BE20" s="18"/>
-      <c r="BF20" s="18"/>
-      <c r="BG20" s="18"/>
+      <c r="BB20" s="16"/>
+      <c r="BC20" s="16"/>
+      <c r="BD20" s="16"/>
+      <c r="BE20" s="16"/>
+      <c r="BF20" s="16"/>
+      <c r="BG20" s="16"/>
     </row>
     <row r="21" spans="11:59" x14ac:dyDescent="0.3">
       <c r="K21" s="2"/>
-      <c r="BB21" s="18"/>
-      <c r="BC21" s="18"/>
-      <c r="BD21" s="18"/>
-      <c r="BE21" s="18"/>
-      <c r="BF21" s="18"/>
-      <c r="BG21" s="18"/>
+      <c r="BB21" s="16"/>
+      <c r="BC21" s="16"/>
+      <c r="BD21" s="16"/>
+      <c r="BE21" s="16"/>
+      <c r="BF21" s="16"/>
+      <c r="BG21" s="16"/>
     </row>
     <row r="22" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB22" s="18"/>
-      <c r="BC22" s="18"/>
-      <c r="BD22" s="18"/>
-      <c r="BE22" s="18"/>
-      <c r="BF22" s="18"/>
-      <c r="BG22" s="18"/>
+      <c r="BB22" s="16"/>
+      <c r="BC22" s="16"/>
+      <c r="BD22" s="16"/>
+      <c r="BE22" s="16"/>
+      <c r="BF22" s="16"/>
+      <c r="BG22" s="16"/>
     </row>
     <row r="23" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB23" s="18"/>
-      <c r="BC23" s="18"/>
-      <c r="BD23" s="18"/>
-      <c r="BE23" s="18"/>
-      <c r="BF23" s="18"/>
-      <c r="BG23" s="18"/>
+      <c r="BB23" s="16"/>
+      <c r="BC23" s="16"/>
+      <c r="BD23" s="16"/>
+      <c r="BE23" s="16"/>
+      <c r="BF23" s="16"/>
+      <c r="BG23" s="16"/>
     </row>
     <row r="24" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB24" s="18"/>
-      <c r="BC24" s="18"/>
-      <c r="BD24" s="18"/>
-      <c r="BE24" s="18"/>
-      <c r="BF24" s="18"/>
-      <c r="BG24" s="18"/>
+      <c r="BB24" s="16"/>
+      <c r="BC24" s="16"/>
+      <c r="BD24" s="16"/>
+      <c r="BE24" s="16"/>
+      <c r="BF24" s="16"/>
+      <c r="BG24" s="16"/>
     </row>
     <row r="25" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB25" s="18"/>
-      <c r="BC25" s="18"/>
-      <c r="BD25" s="18"/>
-      <c r="BE25" s="18"/>
-      <c r="BF25" s="18"/>
-      <c r="BG25" s="18"/>
+      <c r="BB25" s="16"/>
+      <c r="BC25" s="16"/>
+      <c r="BD25" s="16"/>
+      <c r="BE25" s="16"/>
+      <c r="BF25" s="16"/>
+      <c r="BG25" s="16"/>
     </row>
     <row r="26" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB26" s="18"/>
-      <c r="BC26" s="18"/>
-      <c r="BD26" s="18"/>
-      <c r="BE26" s="18"/>
-      <c r="BF26" s="18"/>
-      <c r="BG26" s="18"/>
+      <c r="BB26" s="16"/>
+      <c r="BC26" s="16"/>
+      <c r="BD26" s="16"/>
+      <c r="BE26" s="16"/>
+      <c r="BF26" s="16"/>
+      <c r="BG26" s="16"/>
     </row>
     <row r="27" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB27" s="18"/>
-      <c r="BC27" s="18"/>
-      <c r="BD27" s="18"/>
-      <c r="BE27" s="18"/>
-      <c r="BF27" s="18"/>
-      <c r="BG27" s="18"/>
+      <c r="BB27" s="16"/>
+      <c r="BC27" s="16"/>
+      <c r="BD27" s="16"/>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="16"/>
+      <c r="BG27" s="16"/>
     </row>
     <row r="28" spans="11:59" x14ac:dyDescent="0.3">
-      <c r="BB28" s="18"/>
-      <c r="BC28" s="18"/>
-      <c r="BD28" s="18"/>
-      <c r="BE28" s="18"/>
-      <c r="BF28" s="18"/>
-      <c r="BG28" s="18"/>
+      <c r="BB28" s="16"/>
+      <c r="BC28" s="16"/>
+      <c r="BD28" s="16"/>
+      <c r="BE28" s="16"/>
+      <c r="BF28" s="16"/>
+      <c r="BG28" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lasso feature selection and manual outlier detection
</commit_message>
<xml_diff>
--- a/Code/ML versions.xlsx
+++ b/Code/ML versions.xlsx
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AU5" sqref="AU5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2349,12 +2349,8 @@
       <c r="AW10">
         <v>-0.13</v>
       </c>
-      <c r="BB10" s="16">
-        <v>38596</v>
-      </c>
-      <c r="BC10" s="16">
-        <v>26237</v>
-      </c>
+      <c r="BB10" s="16"/>
+      <c r="BC10" s="16"/>
       <c r="BD10" s="16"/>
       <c r="BE10" s="16"/>
       <c r="BF10" s="16"/>

</xml_diff>